<commit_message>
ajustes do modelo de importacao
</commit_message>
<xml_diff>
--- a/backend/src/utils/Modelo Importacao.xlsx
+++ b/backend/src/utils/Modelo Importacao.xlsx
@@ -302,9 +302,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>845280</xdr:colOff>
+      <xdr:colOff>844920</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>199440</xdr:rowOff>
+      <xdr:rowOff>199080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -318,7 +318,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1832040" cy="2009160"/>
+          <a:ext cx="1831680" cy="2008800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -514,13 +514,13 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="9:9"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="60"/>
@@ -557,8 +557,8 @@
       <c r="C6" s="4"/>
     </row>
     <row r="7" s="6" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -574,8 +574,6 @@
       <c r="O7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
-      <c r="B8" s="0"/>
       <c r="J8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>